<commit_message>
NRC Reactor Status Download and Read CSV
</commit_message>
<xml_diff>
--- a/post9/SE_nuclear_plants.xlsx
+++ b/post9/SE_nuclear_plants.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredkramer/Documents/python/hummingbird/post9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{12C420F0-8FCD-A946-B0E8-29F5F902C5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEB75A0-197E-D848-B15B-29A2E9B8E810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{9CD532EC-D8F3-D04D-84DF-2B259147AA39}"/>
+    <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="16140" xr2:uid="{9CD532EC-D8F3-D04D-84DF-2B259147AA39}"/>
   </bookViews>
   <sheets>
     <sheet name="SE_nuclear_plants" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Plant</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>EIA - daily</t>
+  </si>
+  <si>
+    <t>Began commercial operation 8/31</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/nuclear/reactors/reactorcapacity.php</t>
+  </si>
+  <si>
+    <t>Capacity List</t>
   </si>
 </sst>
 </file>
@@ -442,15 +451,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0944DFFF-4218-B64F-A4CF-6E17B5C50E48}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,13 +476,17 @@
         <v>45184</v>
       </c>
       <c r="G1" s="1">
+        <v>45214</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1">
         <v>45015</v>
       </c>
-      <c r="H1" s="4">
+      <c r="J1" s="4">
         <v>45161</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -489,14 +502,14 @@
       <c r="F2">
         <v>100</v>
       </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -504,7 +517,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>883</v>
+        <v>896</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -512,14 +525,14 @@
       <c r="F3">
         <v>100</v>
       </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -535,14 +548,14 @@
       <c r="F4">
         <v>100</v>
       </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -558,14 +571,14 @@
       <c r="F5">
         <v>100</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>20</v>
       </c>
-      <c r="H5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -581,14 +594,14 @@
       <c r="F6">
         <v>100</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -604,14 +617,14 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-      <c r="H7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>100</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -627,35 +640,42 @@
       <c r="F8">
         <v>100</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>18</v>
       </c>
-      <c r="H8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="L8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="C11">
+        <f>SUM(C2:C8)</f>
+        <v>6948</v>
+      </c>
       <c r="E11">
         <f>SUMPRODUCT($C$2:$C$8, E2:E8)/100</f>
-        <v>6819.8</v>
+        <v>6832.8</v>
       </c>
       <c r="F11">
         <f>SUMPRODUCT($C$2:$C$8, F2:F8)/100</f>
-        <v>5783</v>
-      </c>
-      <c r="G11">
-        <f>SUMPRODUCT($C$2:$C$8, G2:G8)/100</f>
-        <v>4162.66</v>
-      </c>
-      <c r="H11">
-        <f>SUMPRODUCT($C$2:$C$8, H2:H8)/100</f>
-        <v>5785</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5796</v>
+      </c>
+      <c r="I11">
+        <f>SUMPRODUCT($C$2:$C$8, I2:I8)/100</f>
+        <v>4175.66</v>
+      </c>
+      <c r="J11">
+        <f>SUMPRODUCT($C$2:$C$8, J2:J8)/100</f>
+        <v>5798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -665,14 +685,14 @@
       <c r="F12">
         <v>140259</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>96211</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>138102</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E13" s="2">
         <f>E12/24</f>
         <v>6894.583333333333</v>
@@ -681,31 +701,63 @@
         <f>F12/24</f>
         <v>5844.125</v>
       </c>
-      <c r="G13" s="2">
-        <f>G12/24</f>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2">
+        <f>I12/24</f>
         <v>4008.7916666666665</v>
       </c>
-      <c r="H13" s="2">
-        <f>H12/24</f>
+      <c r="J13" s="2">
+        <f>J12/24</f>
         <v>5754.25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E14" s="3">
         <f>E13/E11-1</f>
-        <v>1.0965619715143093E-2</v>
+        <v>9.0421691449087405E-3</v>
       </c>
       <c r="F14" s="3">
         <f>F13/F11-1</f>
-        <v>1.0569773473975363E-2</v>
-      </c>
-      <c r="G14" s="3">
-        <f>G13/G11-1</f>
-        <v>-3.6963944529059156E-2</v>
-      </c>
-      <c r="H14" s="3">
-        <f>H13/H11-1</f>
-        <v>-5.3154710458080956E-3</v>
+        <v>8.3031400966182556E-3</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3">
+        <f>I13/I11-1</f>
+        <v>-3.9962145704710905E-2</v>
+      </c>
+      <c r="J14" s="3">
+        <f>J13/J11-1</f>
+        <v>-7.5457054156605752E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O17">
+        <f>AVERAGE(3.22, 3.75)</f>
+        <v>3.4850000000000003</v>
+      </c>
+      <c r="Q17">
+        <f>AVERAGE(3.22, 3.86)</f>
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <f>O17-2.35</f>
+        <v>1.1350000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <f>O17-2.45</f>
+        <v>1.0350000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
successfully plot % charts (looks terrible)
</commit_message>
<xml_diff>
--- a/post9/SE_nuclear_plants.xlsx
+++ b/post9/SE_nuclear_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredkramer/Documents/python/hummingbird/post9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEB75A0-197E-D848-B15B-29A2E9B8E810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F1834E-A74B-F84E-AE5F-0ABFA86F7906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="16140" xr2:uid="{9CD532EC-D8F3-D04D-84DF-2B259147AA39}"/>
+    <workbookView xWindow="760" yWindow="540" windowWidth="28040" windowHeight="16140" xr2:uid="{9CD532EC-D8F3-D04D-84DF-2B259147AA39}"/>
   </bookViews>
   <sheets>
     <sheet name="SE_nuclear_plants" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates to plant status charts
</commit_message>
<xml_diff>
--- a/post9/SE_nuclear_plants.xlsx
+++ b/post9/SE_nuclear_plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredkramer/Documents/python/hummingbird/post9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F1834E-A74B-F84E-AE5F-0ABFA86F7906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196A9FAE-0CE2-CD49-8620-0B0332452422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="540" windowWidth="28040" windowHeight="16140" xr2:uid="{9CD532EC-D8F3-D04D-84DF-2B259147AA39}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
-  <si>
-    <t>Plant</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>State</t>
   </si>
@@ -71,36 +68,17 @@
     <t>GA</t>
   </si>
   <si>
-    <t>Capacity (MWe)</t>
-  </si>
-  <si>
-    <t>NRC</t>
-  </si>
-  <si>
-    <t>EIA - daily</t>
-  </si>
-  <si>
-    <t>Began commercial operation 8/31</t>
-  </si>
-  <si>
-    <t>https://www.eia.gov/nuclear/reactors/reactorcapacity.php</t>
-  </si>
-  <si>
-    <t>Capacity List</t>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,20 +104,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -451,313 +423,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0944DFFF-4218-B64F-A4CF-6E17B5C50E48}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1">
-        <v>45173</v>
-      </c>
-      <c r="F1" s="1">
-        <v>45184</v>
-      </c>
-      <c r="G1" s="1">
-        <v>45214</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1">
-        <v>45015</v>
-      </c>
-      <c r="J1" s="4">
-        <v>45161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>874</v>
       </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="I2">
-        <v>100</v>
-      </c>
-      <c r="J2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>896</v>
       </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="I3">
-        <v>100</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>876</v>
       </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>100</v>
-      </c>
-      <c r="I4">
-        <v>100</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>883</v>
       </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="I5">
-        <v>20</v>
-      </c>
-      <c r="J5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>1150</v>
       </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>1152</v>
       </c>
-      <c r="E7">
-        <v>90</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>100</v>
-      </c>
-      <c r="J7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>1117</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>100</v>
-      </c>
-      <c r="I8">
-        <v>18</v>
-      </c>
-      <c r="J8">
-        <v>100</v>
-      </c>
-      <c r="L8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <f>SUM(C2:C8)</f>
-        <v>6948</v>
-      </c>
-      <c r="E11">
-        <f>SUMPRODUCT($C$2:$C$8, E2:E8)/100</f>
-        <v>6832.8</v>
-      </c>
-      <c r="F11">
-        <f>SUMPRODUCT($C$2:$C$8, F2:F8)/100</f>
-        <v>5796</v>
-      </c>
-      <c r="I11">
-        <f>SUMPRODUCT($C$2:$C$8, I2:I8)/100</f>
-        <v>4175.66</v>
-      </c>
-      <c r="J11">
-        <f>SUMPRODUCT($C$2:$C$8, J2:J8)/100</f>
-        <v>5798</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12">
-        <v>165470</v>
-      </c>
-      <c r="F12">
-        <v>140259</v>
-      </c>
-      <c r="I12">
-        <v>96211</v>
-      </c>
-      <c r="J12">
-        <v>138102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E13" s="2">
-        <f>E12/24</f>
-        <v>6894.583333333333</v>
-      </c>
-      <c r="F13" s="2">
-        <f>F12/24</f>
-        <v>5844.125</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2">
-        <f>I12/24</f>
-        <v>4008.7916666666665</v>
-      </c>
-      <c r="J13" s="2">
-        <f>J12/24</f>
-        <v>5754.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E14" s="3">
-        <f>E13/E11-1</f>
-        <v>9.0421691449087405E-3</v>
-      </c>
-      <c r="F14" s="3">
-        <f>F13/F11-1</f>
-        <v>8.3031400966182556E-3</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3">
-        <f>I13/I11-1</f>
-        <v>-3.9962145704710905E-2</v>
-      </c>
-      <c r="J14" s="3">
-        <f>J13/J11-1</f>
-        <v>-7.5457054156605752E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="O17">
-        <f>AVERAGE(3.22, 3.75)</f>
-        <v>3.4850000000000003</v>
-      </c>
-      <c r="Q17">
-        <f>AVERAGE(3.22, 3.86)</f>
-        <v>3.54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="O18">
-        <f>O17-2.35</f>
-        <v>1.1350000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="O19">
-        <f>O17-2.45</f>
-        <v>1.0350000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>